<commit_message>
Translation FRA -> ENG for the Summary file
</commit_message>
<xml_diff>
--- a/Data/Markerless/Method8/Summary.xlsx
+++ b/Data/Markerless/Method8/Summary.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Recherche\Github\challenge_markerless\Method8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Recherche\Github\Benchmarking_markerless\Data\Markerless\Method8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E82473-1EA5-4E15-8A37-39767CC815AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D3EF5-30E3-4B6E-B66E-CBC8FAF3197C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Méthode" sheetId="1" r:id="rId1"/>
-    <sheet name="Résultats" sheetId="2" r:id="rId2"/>
+    <sheet name="Method" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -627,6 +627,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,9 +650,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1025,7 +1025,7 @@
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="35" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89299E4-08D1-44F4-A16E-5652B9F53E8D}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1058,26 +1058,26 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="35" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="35" t="s">
+      <c r="F3" s="37"/>
+      <c r="G3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="35" t="s">
+      <c r="H3" s="37"/>
+      <c r="I3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37" t="s">
+      <c r="J3" s="37"/>
+      <c r="K3" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="36"/>
+      <c r="L3" s="37"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
@@ -1114,10 +1114,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="41"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="17" t="s">
         <v>29</v>
       </c>
@@ -1150,7 +1150,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -1188,7 +1188,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="21" t="s">
         <v>3</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="21" t="s">
         <v>4</v>
       </c>
@@ -1260,7 +1260,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="21" t="s">
         <v>2</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="21" t="s">
         <v>6</v>
       </c>
@@ -1368,7 +1368,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="21" t="s">
         <v>7</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
       </c>
@@ -1440,7 +1440,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="22" t="s">
         <v>10</v>
       </c>

</xml_diff>